<commit_message>
Done "Overall task progress chart"
</commit_message>
<xml_diff>
--- a/excel/Management/Project Management Dashboard.xlsx
+++ b/excel/Management/Project Management Dashboard.xlsx
@@ -2,21 +2,45 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekaterinakuzmina/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekaterinakuzmina/Desktop/repos/analysis/excel/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4830ADBE-17FD-314F-94FC-27F4BC096D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946EE12A-C911-0848-A143-F3B5ADEE26CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="5000" windowWidth="29040" windowHeight="16440" tabRatio="664" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
+    <workbookView xWindow="12420" yWindow="4840" windowWidth="35560" windowHeight="19480" tabRatio="664" activeTab="2" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Workings" sheetId="3" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Workings!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Workings!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Workings!$B$2:$B$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="14" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="39">
   <si>
     <t>Project</t>
   </si>
@@ -123,15 +147,43 @@
   <si>
     <t>Task 10</t>
   </si>
+  <si>
+    <t>Project Management Dashboard</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual </t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Total Tasks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +198,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="30"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -163,23 +226,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -247,8 +344,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="No Border" pivot="0" table="0" count="10" xr9:uid="{EEEA172B-89F3-489D-B80E-D598FE9BFA19}">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
-      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -516,6 +613,2349 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>O</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>VERALL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> TASK PROGRESS</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.4751570601697389E-2"/>
+          <c:y val="4.8514931305333041E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not Started</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CZ"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1240-D14F-BED3-93DD828B8161}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In Progress</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CZ"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1240-D14F-BED3-93DD828B8161}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Completed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-CZ"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1240-D14F-BED3-93DD828B8161}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="100"/>
+        <c:axId val="1449249600"/>
+        <c:axId val="1449251248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1449249600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1449251248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1449251248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1449249600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.6577274592088418E-2"/>
+          <c:y val="0.39863364838074072"/>
+          <c:w val="0.71928707534439551"/>
+          <c:h val="0.16736345456817897"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>740834</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>31749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>675810</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>148165</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52DADD6-19BC-B948-991F-C516C2C68D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44968.546006828707" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="40" xr:uid="{2E8955EA-A8BA-5048-B79E-974F2C9DA3E0}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Project" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Gemini"/>
+        <s v="Orion"/>
+        <s v="Vega"/>
+        <s v="Delta"/>
+        <s v="Alpha"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Task" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Task 1"/>
+        <s v="Task 2"/>
+        <s v="Task 3"/>
+        <s v="Task 4"/>
+        <s v="Task 5"/>
+        <s v="Task 6"/>
+        <s v="Task 7"/>
+        <s v="Task 8"/>
+        <s v="Task 9"/>
+        <s v="Task 10"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Manager" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Hirsch"/>
+        <s v="Samora"/>
+        <s v="McFay"/>
+        <s v="Wood"/>
+        <s v="Ladd"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Start Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-02-17T00:00:00" maxDate="2020-03-03T00:00:00" count="11">
+        <d v="2020-02-17T00:00:00"/>
+        <d v="2020-02-18T00:00:00"/>
+        <d v="2020-02-21T00:00:00"/>
+        <d v="2020-02-20T00:00:00"/>
+        <d v="2020-02-24T00:00:00"/>
+        <d v="2020-02-25T00:00:00"/>
+        <d v="2020-02-27T00:00:00"/>
+        <d v="2020-02-26T00:00:00"/>
+        <d v="2020-02-28T00:00:00"/>
+        <d v="2020-03-02T00:00:00"/>
+        <d v="2020-02-19T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Duration" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="10" count="8">
+        <n v="5"/>
+        <n v="6"/>
+        <n v="10"/>
+        <n v="9"/>
+        <n v="4"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="End Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-02-19T00:00:00" maxDate="2020-03-14T00:00:00" count="15">
+        <d v="2020-02-21T00:00:00"/>
+        <d v="2020-02-24T00:00:00"/>
+        <d v="2020-03-02T00:00:00"/>
+        <d v="2020-03-04T00:00:00"/>
+        <d v="2020-02-20T00:00:00"/>
+        <d v="2020-02-27T00:00:00"/>
+        <d v="2020-02-28T00:00:00"/>
+        <d v="2020-03-05T00:00:00"/>
+        <d v="2020-02-26T00:00:00"/>
+        <d v="2020-03-06T00:00:00"/>
+        <d v="2020-02-19T00:00:00"/>
+        <d v="2020-03-03T00:00:00"/>
+        <d v="2020-03-12T00:00:00"/>
+        <d v="2020-03-13T00:00:00"/>
+        <d v="2020-03-10T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Days completed" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="8" count="8">
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="1"/>
+        <n v="0"/>
+        <n v="7"/>
+        <n v="5"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Progress" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1" count="19">
+        <n v="0.4"/>
+        <n v="0.5"/>
+        <n v="0.33333333333333331"/>
+        <n v="0.25"/>
+        <n v="0"/>
+        <n v="0.42857142857142855"/>
+        <n v="0.1111111111111111"/>
+        <n v="1"/>
+        <n v="0.44444444444444442"/>
+        <n v="0.83333333333333337"/>
+        <n v="0.8"/>
+        <n v="0.2857142857142857"/>
+        <n v="0.66666666666666663"/>
+        <n v="0.88888888888888884"/>
+        <n v="0.2"/>
+        <n v="0.625"/>
+        <n v="0.3"/>
+        <n v="0.375"/>
+        <n v="0.6"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Budget" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="50000" maxValue="990000"/>
+    </cacheField>
+    <cacheField name="Actual" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="807069"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="218000"/>
+    <n v="97337"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="393000"/>
+    <n v="177440"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="86000"/>
+    <n v="31046"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="732000"/>
+    <n v="261324"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="492000"/>
+    <n v="116850"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="188000"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="180000"/>
+    <n v="79380"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="582000"/>
+    <n v="195231"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="562000"/>
+    <n v="74746"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="416000"/>
+    <n v="175015"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="7"/>
+    <n v="293000"/>
+    <n v="273001"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="224000"/>
+    <n v="57910"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="978000"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="932000"/>
+    <n v="379157"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="854000"/>
+    <n v="322812"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="81000"/>
+    <n v="38461"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="9"/>
+    <n v="169000"/>
+    <n v="136468"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="61000"/>
+    <n v="12078"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="645000"/>
+    <n v="273048"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="68000"/>
+    <n v="64987"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="839000"/>
+    <n v="406974"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="10"/>
+    <n v="729000"/>
+    <n v="487139"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="826000"/>
+    <n v="298186"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="11"/>
+    <n v="895000"/>
+    <n v="280583"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="8"/>
+    <x v="7"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="341000"/>
+    <n v="129785"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="7"/>
+    <x v="13"/>
+    <n v="787000"/>
+    <n v="727188"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="14"/>
+    <n v="228000"/>
+    <n v="47880"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="147000"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="15"/>
+    <n v="338000"/>
+    <n v="205123"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="16"/>
+    <n v="857000"/>
+    <n v="305949"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="602000"/>
+    <n v="322371"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="990000"/>
+    <n v="451440"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="6"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="17"/>
+    <n v="96000"/>
+    <n v="32256"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="513000"/>
+    <n v="226233"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="18"/>
+    <n v="616000"/>
+    <n v="401579"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="817000"/>
+    <n v="807069"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="372000"/>
+    <n v="173166"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="14"/>
+    <n v="50000"/>
+    <n v="8400"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="16"/>
+    <n v="807000"/>
+    <n v="262679"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="8"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="691000"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3D4DA184-71F2-1746-9ED0-A1386861AAD3}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A6:J47" firstHeaderRow="0" firstDataRow="1" firstDataCol="8"/>
+  <pivotFields count="10">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="9"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="15">
+        <item x="10"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="11"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="7"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" numFmtId="9" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="19">
+        <item x="4"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="16"/>
+        <item x="2"/>
+        <item x="17"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="18"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="7"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="8">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+    <field x="5"/>
+    <field x="4"/>
+    <field x="6"/>
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="41">
+    <i>
+      <x/>
+      <x/>
+      <x v="2"/>
+      <x v="9"/>
+      <x v="12"/>
+      <x v="5"/>
+      <x v="3"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="4"/>
+      <x v="10"/>
+      <x v="13"/>
+      <x v="6"/>
+      <x v="4"/>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="1"/>
+      <x v="3"/>
+      <x v="4"/>
+      <x v="2"/>
+      <x v="3"/>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x/>
+      <x v="2"/>
+      <x v="2"/>
+      <x/>
+      <x v="3"/>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="3"/>
+      <x v="4"/>
+      <x v="7"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x v="2"/>
+      <x v="5"/>
+      <x v="11"/>
+      <x v="7"/>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="4"/>
+      <x v="5"/>
+      <x v="11"/>
+      <x v="7"/>
+      <x v="3"/>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+      <x v="1"/>
+      <x v="5"/>
+      <x v="4"/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x/>
+      <x v="10"/>
+      <x v="13"/>
+      <x v="6"/>
+      <x v="7"/>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="3"/>
+      <x v="10"/>
+      <x v="14"/>
+      <x v="7"/>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="2"/>
+      <x/>
+      <x v="1"/>
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="4"/>
+      <x v="2"/>
+      <x v="6"/>
+      <x v="5"/>
+      <x v="5"/>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="1"/>
+      <x v="5"/>
+      <x v="11"/>
+      <x v="7"/>
+      <x v="3"/>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x/>
+      <x v="6"/>
+      <x v="8"/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+      <x v="6"/>
+      <x v="6"/>
+      <x v="1"/>
+      <x v="2"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x/>
+      <x v="2"/>
+      <x v="2"/>
+      <x v="2"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="5"/>
+      <x v="7"/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="3"/>
+      <x/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="2"/>
+      <x v="1"/>
+      <x v="7"/>
+      <x v="7"/>
+      <x v="4"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="4"/>
+      <x v="4"/>
+      <x v="9"/>
+      <x v="6"/>
+      <x v="3"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x/>
+      <x v="3"/>
+      <x v="5"/>
+      <x v="3"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="6"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+      <x v="2"/>
+      <x v="5"/>
+      <x v="6"/>
+      <x v="2"/>
+      <x v="2"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+      <x v="4"/>
+      <x v="5"/>
+      <x v="10"/>
+      <x v="6"/>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+      <x v="4"/>
+      <x v="4"/>
+      <x v="6"/>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x/>
+      <x/>
+      <x/>
+      <x v="3"/>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="3"/>
+      <x/>
+      <x v="5"/>
+      <x v="6"/>
+      <x v="4"/>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="2"/>
+      <x v="1"/>
+      <x v="5"/>
+      <x v="5"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="6"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="1"/>
+      <x v="4"/>
+      <x v="4"/>
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x/>
+      <x v="4"/>
+      <x v="6"/>
+      <x v="3"/>
+      <x v="3"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+      <x v="5"/>
+      <x v="7"/>
+      <x v="3"/>
+      <x v="5"/>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+      <x v="2"/>
+      <x v="6"/>
+      <x v="6"/>
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+      <x v="4"/>
+      <x v="8"/>
+      <x v="11"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+      <x/>
+      <x/>
+      <x v="6"/>
+      <x v="7"/>
+      <x v="5"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="3"/>
+      <x v="4"/>
+      <x v="5"/>
+      <x v="2"/>
+      <x v="4"/>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="2"/>
+      <x v="5"/>
+      <x v="8"/>
+      <x v="4"/>
+      <x v="3"/>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="4"/>
+      <x v="7"/>
+      <x v="10"/>
+      <x v="4"/>
+      <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="1"/>
+      <x v="9"/>
+      <x v="8"/>
+      <x/>
+      <x v="2"/>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Budget " fld="8" baseField="0" baseItem="0" numFmtId="3"/>
+    <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="9">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5D3C948-3701-4929-B04F-010B6EBC2A77}" name="Table1" displayName="Table1" ref="A1:J41" totalsRowShown="0">
   <autoFilter ref="A1:J41" xr:uid="{7E21CF9F-AD78-47F7-B4FB-8E64E3714907}"/>
@@ -523,19 +2963,19 @@
     <tableColumn id="1" xr3:uid="{4ADE78FA-797E-461B-818D-4E6F917859D6}" name="Project"/>
     <tableColumn id="2" xr3:uid="{F9E92030-47E5-4A86-AB73-A1AA5209CD55}" name="Task"/>
     <tableColumn id="3" xr3:uid="{643837EC-0E87-4517-8311-405E12C9047D}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{D2195ACD-57B1-4029-9C54-9ACCE862FA18}" name="Start Date" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D2195ACD-57B1-4029-9C54-9ACCE862FA18}" name="Start Date" dataDxfId="10"/>
     <tableColumn id="5" xr3:uid="{A5BEB9B6-A13C-4735-8C93-943512962E1A}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{9A8390CA-408A-41FE-A909-4D1F9E77E3F2}" name="End Date" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{9A8390CA-408A-41FE-A909-4D1F9E77E3F2}" name="End Date" dataDxfId="9">
       <calculatedColumnFormula>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{06B5F73C-C916-4EC2-88F2-098623EC6F35}" name="Days completed" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{704AC253-E86F-4A7F-BD63-4569C494A728}" name="Progress" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{06B5F73C-C916-4EC2-88F2-098623EC6F35}" name="Days completed" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{704AC253-E86F-4A7F-BD63-4569C494A728}" name="Progress" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Days completed]]/Table1[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{459C1C51-A35C-450A-B0F0-EA7E00C33AA1}" name="Budget" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{CC94112E-5637-4797-9BDD-BFCC8197D1AB}" name="Actual" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{459C1C51-A35C-450A-B0F0-EA7E00C33AA1}" name="Budget" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{CC94112E-5637-4797-9BDD-BFCC8197D1AB}" name="Actual" dataDxfId="5"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -839,7 +3279,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2296,14 +4736,1326 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E827AB40-3701-514F-9CCF-DEF1B95D471A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F759922C-CDE1-CC48-BA2D-DA4DF947C12C}">
+  <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(Dashboard!H7:H46,"="&amp;0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIFS(Dashboard!H7:H46,"&lt;&gt;"&amp;0,Dashboard!H7:H46,"&lt;"&amp;1)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(Dashboard!H7:H46,"="&amp;1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10">
+        <f>B2+B3</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <f>B4+B5</f>
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E827AB40-3701-514F-9CCF-DEF1B95D471A}">
+  <dimension ref="A1:R47"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43889</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43900</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="I7" s="9">
+        <v>96000</v>
+      </c>
+      <c r="J7" s="3">
+        <v>32256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43892</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43902</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I8" s="3">
+        <v>513000</v>
+      </c>
+      <c r="J8" s="3">
+        <v>226233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43881</v>
+      </c>
+      <c r="E9" s="1">
+        <v>43887</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>616000</v>
+      </c>
+      <c r="J9" s="3">
+        <v>401579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43880</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43882</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>817000</v>
+      </c>
+      <c r="J10" s="3">
+        <v>807069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43882</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43892</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I11" s="3">
+        <v>372000</v>
+      </c>
+      <c r="J11" s="3">
+        <v>173166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43896</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>50000</v>
+      </c>
+      <c r="J12" s="3">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43896</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>807000</v>
+      </c>
+      <c r="J13" s="3">
+        <v>262679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43887</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>691000</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43892</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43902</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3">
+        <v>8</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="I15" s="3">
+        <v>787000</v>
+      </c>
+      <c r="J15" s="3">
+        <v>727188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43892</v>
+      </c>
+      <c r="E16" s="1">
+        <v>43903</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>228000</v>
+      </c>
+      <c r="J16" s="3">
+        <v>47880</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E17" s="1">
+        <v>43881</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>147000</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43880</v>
+      </c>
+      <c r="E18" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="I18" s="3">
+        <v>338000</v>
+      </c>
+      <c r="J18" s="3">
+        <v>205123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E19" s="1">
+        <v>43896</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>857000</v>
+      </c>
+      <c r="J19" s="3">
+        <v>305949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43886</v>
+      </c>
+      <c r="E20" s="1">
+        <v>43893</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="3">
+        <v>602000</v>
+      </c>
+      <c r="J20" s="3">
+        <v>322371</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43886</v>
+      </c>
+      <c r="E21" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>990000</v>
+      </c>
+      <c r="J21" s="3">
+        <v>451440</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E22" s="1">
+        <v>43882</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I22" s="3">
+        <v>218000</v>
+      </c>
+      <c r="J22" s="3">
+        <v>97337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E23" s="1">
+        <v>43892</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="3">
+        <v>416000</v>
+      </c>
+      <c r="J23" s="3">
+        <v>175015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E24" s="1">
+        <v>43885</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="3">
+        <v>393000</v>
+      </c>
+      <c r="J24" s="3">
+        <v>177440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43879</v>
+      </c>
+      <c r="E25" s="1">
+        <v>43892</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>86000</v>
+      </c>
+      <c r="J25" s="3">
+        <v>31046</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="1">
+        <v>43882</v>
+      </c>
+      <c r="E26" s="1">
+        <v>43894</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I26" s="3">
+        <v>732000</v>
+      </c>
+      <c r="J26" s="3">
+        <v>261324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E27" s="1">
+        <v>43881</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I27" s="3">
+        <v>492000</v>
+      </c>
+      <c r="J27" s="3">
+        <v>116850</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1">
+        <v>43881</v>
+      </c>
+      <c r="E28" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>188000</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1">
+        <v>43881</v>
+      </c>
+      <c r="E29" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I29" s="3">
+        <v>180000</v>
+      </c>
+      <c r="J29" s="3">
+        <v>79380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E30" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2</v>
+      </c>
+      <c r="H30" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I30" s="3">
+        <v>582000</v>
+      </c>
+      <c r="J30" s="3">
+        <v>195231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E31" s="1">
+        <v>43895</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="I31" s="3">
+        <v>562000</v>
+      </c>
+      <c r="J31" s="3">
+        <v>74746</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="1">
+        <v>43879</v>
+      </c>
+      <c r="E32" s="1">
+        <v>43887</v>
+      </c>
+      <c r="F32">
+        <v>7</v>
+      </c>
+      <c r="G32" s="3">
+        <v>7</v>
+      </c>
+      <c r="H32" s="7">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3">
+        <v>293000</v>
+      </c>
+      <c r="J32" s="3">
+        <v>273001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43880</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>68000</v>
+      </c>
+      <c r="J33" s="3">
+        <v>64987</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E34" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="G34" s="3">
+        <v>4</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I34" s="3">
+        <v>224000</v>
+      </c>
+      <c r="J34" s="3">
+        <v>57910</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="1">
+        <v>43879</v>
+      </c>
+      <c r="E35" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>978000</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43881</v>
+      </c>
+      <c r="E36" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I36" s="3">
+        <v>932000</v>
+      </c>
+      <c r="J36" s="3">
+        <v>379157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1">
+        <v>43882</v>
+      </c>
+      <c r="E37" s="1">
+        <v>43887</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I37" s="3">
+        <v>854000</v>
+      </c>
+      <c r="J37" s="3">
+        <v>322812</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1">
+        <v>43882</v>
+      </c>
+      <c r="E38" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38" s="3">
+        <v>3</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="3">
+        <v>81000</v>
+      </c>
+      <c r="J38" s="3">
+        <v>38461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E39" s="1">
+        <v>43892</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39" s="3">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I39" s="3">
+        <v>169000</v>
+      </c>
+      <c r="J39" s="3">
+        <v>136468</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="1">
+        <v>43886</v>
+      </c>
+      <c r="E40" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I40" s="3">
+        <v>61000</v>
+      </c>
+      <c r="J40" s="3">
+        <v>12078</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="1">
+        <v>43888</v>
+      </c>
+      <c r="E41" s="1">
+        <v>43896</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41" s="3">
+        <v>3</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I41" s="3">
+        <v>645000</v>
+      </c>
+      <c r="J41" s="3">
+        <v>273048</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="1">
+        <v>43878</v>
+      </c>
+      <c r="E42" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42" s="3">
+        <v>5</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="3">
+        <v>839000</v>
+      </c>
+      <c r="J42" s="3">
+        <v>406974</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="1">
+        <v>43882</v>
+      </c>
+      <c r="E43" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43" s="3">
+        <v>4</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="I43" s="3">
+        <v>729000</v>
+      </c>
+      <c r="J43" s="3">
+        <v>487139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="1">
+        <v>43885</v>
+      </c>
+      <c r="E44" s="1">
+        <v>43893</v>
+      </c>
+      <c r="F44">
+        <v>7</v>
+      </c>
+      <c r="G44" s="3">
+        <v>3</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I44" s="3">
+        <v>826000</v>
+      </c>
+      <c r="J44" s="3">
+        <v>298186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="1">
+        <v>43887</v>
+      </c>
+      <c r="E45" s="1">
+        <v>43895</v>
+      </c>
+      <c r="F45">
+        <v>7</v>
+      </c>
+      <c r="G45" s="3">
+        <v>2</v>
+      </c>
+      <c r="H45" s="7">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="I45" s="3">
+        <v>895000</v>
+      </c>
+      <c r="J45" s="3">
+        <v>280583</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1">
+        <v>43889</v>
+      </c>
+      <c r="E46" s="1">
+        <v>43893</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46" s="3">
+        <v>2</v>
+      </c>
+      <c r="H46" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I46" s="3">
+        <v>341000</v>
+      </c>
+      <c r="J46" s="3">
+        <v>129785</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="3">
+        <v>19695000</v>
+      </c>
+      <c r="J47" s="3">
+        <v>8340291</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>